<commit_message>
Zeigerdiagramm aktiviert, Vorlagen bereitgestellt (Excel), Handbuch erstellt
</commit_message>
<xml_diff>
--- a/Vorlage (FF) - Import Excel-Datei in Datenbank.xlsx
+++ b/Vorlage (FF) - Import Excel-Datei in Datenbank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genesis\Desktop\ilias Generator - Projekt\Datenbank_Export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genesis\Documents\GitHub\ILIAS---Test-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="217">
   <si>
     <t>question_difficulty</t>
   </si>
@@ -669,105 +669,6 @@
   </si>
   <si>
     <t>$r1</t>
-  </si>
-  <si>
-    <t>7.11.02 b Zylinderspule</t>
-  </si>
-  <si>
-    <t>Berechnung der magnetischen Flussdichte B in einer luftgefüllten Spule</t>
-  </si>
-  <si>
-    <t>Eine Zylinderspule wird mit einem Strom von //I/// = $v1 mA betrieben. Sie hat //N/// = $v2 Windungen und ist $v3 cm lang. Bestimmen Sie die magnetische Feldstärke //H/// im Inneren der luftgefüllten Spule.
-//B/// = $r1 µT</t>
-  </si>
-  <si>
-    <t>1000000*($v2*$v1*10^-3)/($v3*10^-2)*1,256637*10^-6</t>
-  </si>
-  <si>
-    <t>Leiter einer Spule</t>
-  </si>
-  <si>
-    <t>7.11.06 Kraft auf Leiter im Magnetfeld</t>
-  </si>
-  <si>
-    <t>Berechnung der Lorenzkraft auf einen Strom durchflossenen Leiter in einer Spule</t>
-  </si>
-  <si>
-    <t>Eine Zylinderspule mit //N/// = $v1 Windungen und der Länge \(l_S =\) $v2 cm wird von einem Spulenstrom \(I_S =\) $v3 A durchflossen. In der Mitte der Spule befindet sich ein Leiter, der vom Strom \(I_L =\) $v4 A durchströmt wird. Der Leiter ist \(l_L =\) $v5 cm lang. Bestimmen Sie die Kraft auf den Leiter, die das äußere Magnetfeld verursacht.
-//F_L/// = $r1 N</t>
-  </si>
-  <si>
-    <t>1000*(($v3*$v1)/($v2*10^-2))*(1,256637*10^-6)*$v4*($v5*10^-2)</t>
-  </si>
-  <si>
-    <t>$v4</t>
-  </si>
-  <si>
-    <t>$v5</t>
-  </si>
-  <si>
-    <t>Permeabilität von verschiedenen Materialien</t>
-  </si>
-  <si>
-    <t>7.11.03 a Permeabilitätszahl von Eisen</t>
-  </si>
-  <si>
-    <t>magnetische Feldstärke ausrechnen</t>
-  </si>
-  <si>
-    <t>Betrachten Sie eine Kreisringspule mit dem mittleren Durchmesser //D/// = $v1 cm und dem Querschnitt $v1 cm^2 . Sie hat $v3 Windungen und ist mit Schmiedestahl gefüllt (Magnetisierungskurve für kaltgewalztes Elektroblech V400-50 A in Abbildung). Welche magnetische Feldstärke //H/// herrscht auf dem Feldlinienring des Durchmessers //D///, wenn ein Strom von //I/// = $v4 A fließt?
-//H/// = $r1 A/m</t>
-  </si>
-  <si>
-    <t>0,001*($v3*$v4)/(pi*$v1*10^-2)+$v1-$v1</t>
-  </si>
-  <si>
-    <t>Bilder/Permeabilitätszahl von Eisen (Skript).png</t>
-  </si>
-  <si>
-    <t>Primär- und Sekundärwerte ausrechnen</t>
-  </si>
-  <si>
-    <t>8.9.03 a Idealer Transformator</t>
-  </si>
-  <si>
-    <t>Spannung auf der Primärseite berechnen</t>
-  </si>
-  <si>
-    <t>Ein idealer Transformator  (in der Literatur auch genannt idealer Übertrager) hat ein Übersetzungsverhältnis von \(\text{ü}=\frac{N_2}{N_1}=\) $v1. Eine Sekundärspannung von //U_2/// = $v2 V tritt auf. Berechnen Sie den Effektivwert der Primärspannung.
-//U_1/// = $r1 V</t>
-  </si>
-  <si>
-    <t>$v2/$v1</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>8.9.03 b Idealer Transformator</t>
-  </si>
-  <si>
-    <t>Strom auf der Sekundärseite berechnen</t>
-  </si>
-  <si>
-    <t>Ein idealer Transformator  (in der Literatur auch genannt idealer Übertrager) hat ein Übersetzungsverhältnis von \(\text{ü}=\frac{N_2}{N_1}=\) = $v3. Eine Sekundärspannung von //U_2/// = $v2 V tritt auf, wenn man auf der Sekundärseite einen Widerstand von //R_2/// = $v1 &amp;Omega; anschließt. Berechnen Sie den Effektivwert des Sekundärstroms.
-//I_2/// = $r1 A</t>
-  </si>
-  <si>
-    <t>($v1/$v2)+$v3-$v3</t>
-  </si>
-  <si>
-    <t>8.9.03 c Idealer Transformator</t>
-  </si>
-  <si>
-    <t>Strom auf der Primärseite berechnen</t>
-  </si>
-  <si>
-    <t>Ein idealer Transformator  (in der Literatur auch genannt idealer Übertrager) hat ein Übersetzungsverhältnis von //ü/// = $v1. Eine Sekundärspannung von //U_2/// = $v2 V tritt auf, wenn man auf der Sekundärseite einen Widerstand von //R_2/// = $v3 &amp;Omega; anschließt. Berechnen Sie den Effektivwert des Primärstroms.
-//I_1/// = $r1 mA</t>
-  </si>
-  <si>
-    <t>1000*($v2/$v3)*$v1</t>
   </si>
   <si>
     <t>Bild1</t>
@@ -1143,13 +1044,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GH9"/>
+  <dimension ref="A1:GH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="FU12" sqref="FU12"/>
+    <sheetView tabSelected="1" topLeftCell="FG1" workbookViewId="0">
+      <selection activeCell="FW2" sqref="FW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="177" max="177" width="17.28515625" customWidth="1"/>
+    <col min="178" max="178" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:190" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1977,7 +1882,7 @@
       <c r="FS2" s="2"/>
       <c r="FT2" s="2"/>
       <c r="FU2" s="2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="FV2" s="2" t="s">
         <v>202</v>
@@ -2237,7 +2142,7 @@
       <c r="FS3" s="2"/>
       <c r="FT3" s="2"/>
       <c r="FU3" s="2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="FV3" s="2" t="s">
         <v>202</v>
@@ -2263,1574 +2168,6 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R4" s="2">
-        <v>10</v>
-      </c>
-      <c r="S4" s="2">
-        <v>80</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X4" s="2">
-        <v>1000</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>5000</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>10</v>
-      </c>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>10</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>50</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="2"/>
-      <c r="AT4" s="2"/>
-      <c r="AU4" s="2"/>
-      <c r="AV4" s="2"/>
-      <c r="AW4" s="2"/>
-      <c r="AX4" s="2"/>
-      <c r="AY4" s="2"/>
-      <c r="AZ4" s="2"/>
-      <c r="BA4" s="2"/>
-      <c r="BB4" s="2"/>
-      <c r="BC4" s="2"/>
-      <c r="BD4" s="2"/>
-      <c r="BE4" s="2"/>
-      <c r="BF4" s="2"/>
-      <c r="BG4" s="2"/>
-      <c r="BH4" s="2"/>
-      <c r="BI4" s="2"/>
-      <c r="BJ4" s="2"/>
-      <c r="BK4" s="2"/>
-      <c r="BL4" s="2"/>
-      <c r="BM4" s="2"/>
-      <c r="BN4" s="2"/>
-      <c r="BO4" s="2"/>
-      <c r="BP4" s="2"/>
-      <c r="BQ4" s="2"/>
-      <c r="BR4" s="2"/>
-      <c r="BS4" s="2"/>
-      <c r="BT4" s="2"/>
-      <c r="BU4" s="2"/>
-      <c r="BV4" s="2"/>
-      <c r="BW4" s="2"/>
-      <c r="BX4" s="2"/>
-      <c r="BY4" s="2"/>
-      <c r="BZ4" s="2"/>
-      <c r="CA4" s="2"/>
-      <c r="CB4" s="2"/>
-      <c r="CC4" s="2"/>
-      <c r="CD4" s="2"/>
-      <c r="CE4" s="2"/>
-      <c r="CF4" s="2"/>
-      <c r="CG4" s="2"/>
-      <c r="CH4" s="2"/>
-      <c r="CI4" s="2"/>
-      <c r="CJ4" s="2"/>
-      <c r="CK4" s="2"/>
-      <c r="CL4" s="2"/>
-      <c r="CM4" s="2"/>
-      <c r="CN4" s="2"/>
-      <c r="CO4" s="2"/>
-      <c r="CP4" s="2"/>
-      <c r="CQ4" s="2"/>
-      <c r="CR4" s="2"/>
-      <c r="CS4" s="2"/>
-      <c r="CT4" s="2"/>
-      <c r="CU4" s="2"/>
-      <c r="CV4" s="2"/>
-      <c r="CW4" s="2"/>
-      <c r="CX4" s="2"/>
-      <c r="CY4" s="2"/>
-      <c r="CZ4" s="2"/>
-      <c r="DA4" s="2"/>
-      <c r="DB4" s="2"/>
-      <c r="DC4" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD4" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE4" s="2">
-        <v>10</v>
-      </c>
-      <c r="DF4" s="2">
-        <v>9</v>
-      </c>
-      <c r="DG4" s="2">
-        <v>5</v>
-      </c>
-      <c r="DH4" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI4" s="2"/>
-      <c r="DJ4" s="2"/>
-      <c r="DK4" s="2"/>
-      <c r="DL4" s="2"/>
-      <c r="DM4" s="2"/>
-      <c r="DN4" s="2"/>
-      <c r="DO4" s="2"/>
-      <c r="DP4" s="2"/>
-      <c r="DQ4" s="2"/>
-      <c r="DR4" s="2"/>
-      <c r="DS4" s="2"/>
-      <c r="DT4" s="2"/>
-      <c r="DU4" s="2"/>
-      <c r="DV4" s="2"/>
-      <c r="DW4" s="2"/>
-      <c r="DX4" s="2"/>
-      <c r="DY4" s="2"/>
-      <c r="DZ4" s="2"/>
-      <c r="EA4" s="2"/>
-      <c r="EB4" s="2"/>
-      <c r="EC4" s="2"/>
-      <c r="ED4" s="2"/>
-      <c r="EE4" s="2"/>
-      <c r="EF4" s="2"/>
-      <c r="EG4" s="2"/>
-      <c r="EH4" s="2"/>
-      <c r="EI4" s="2"/>
-      <c r="EJ4" s="2"/>
-      <c r="EK4" s="2"/>
-      <c r="EL4" s="2"/>
-      <c r="EM4" s="2"/>
-      <c r="EN4" s="2"/>
-      <c r="EO4" s="2"/>
-      <c r="EP4" s="2"/>
-      <c r="EQ4" s="2"/>
-      <c r="ER4" s="2"/>
-      <c r="ES4" s="2"/>
-      <c r="ET4" s="2"/>
-      <c r="EU4" s="2"/>
-      <c r="EV4" s="2"/>
-      <c r="EW4" s="2"/>
-      <c r="EX4" s="2"/>
-      <c r="EY4" s="2"/>
-      <c r="EZ4" s="2"/>
-      <c r="FA4" s="2"/>
-      <c r="FB4" s="2"/>
-      <c r="FC4" s="2"/>
-      <c r="FD4" s="2"/>
-      <c r="FE4" s="2"/>
-      <c r="FF4" s="2"/>
-      <c r="FG4" s="2"/>
-      <c r="FH4" s="2"/>
-      <c r="FI4" s="2"/>
-      <c r="FJ4" s="2"/>
-      <c r="FK4" s="2"/>
-      <c r="FL4" s="2"/>
-      <c r="FM4" s="2"/>
-      <c r="FN4" s="2"/>
-      <c r="FO4" s="2"/>
-      <c r="FP4" s="2"/>
-      <c r="FQ4" s="2"/>
-      <c r="FR4" s="2"/>
-      <c r="FS4" s="2"/>
-      <c r="FT4" s="2"/>
-      <c r="FU4" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="FV4" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="FW4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="FX4" s="2"/>
-      <c r="FY4" s="2"/>
-      <c r="FZ4" s="2"/>
-      <c r="GA4" s="2"/>
-      <c r="GB4" s="2"/>
-      <c r="GC4" s="2"/>
-      <c r="GD4" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE4" s="2"/>
-      <c r="GF4" s="2"/>
-      <c r="GG4" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="GH4" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="S5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>100</v>
-      </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X5" s="2">
-        <v>5</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>50</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>11</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>30</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="2"/>
-      <c r="AO5" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="AP5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="2">
-        <v>20</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="2"/>
-      <c r="AU5" s="2"/>
-      <c r="AV5" s="2"/>
-      <c r="AW5" s="2"/>
-      <c r="AX5" s="2"/>
-      <c r="AY5" s="2"/>
-      <c r="AZ5" s="2"/>
-      <c r="BA5" s="2"/>
-      <c r="BB5" s="2"/>
-      <c r="BC5" s="2"/>
-      <c r="BD5" s="2"/>
-      <c r="BE5" s="2"/>
-      <c r="BF5" s="2"/>
-      <c r="BG5" s="2"/>
-      <c r="BH5" s="2"/>
-      <c r="BI5" s="2"/>
-      <c r="BJ5" s="2"/>
-      <c r="BK5" s="2"/>
-      <c r="BL5" s="2"/>
-      <c r="BM5" s="2"/>
-      <c r="BN5" s="2"/>
-      <c r="BO5" s="2"/>
-      <c r="BP5" s="2"/>
-      <c r="BQ5" s="2"/>
-      <c r="BR5" s="2"/>
-      <c r="BS5" s="2"/>
-      <c r="BT5" s="2"/>
-      <c r="BU5" s="2"/>
-      <c r="BV5" s="2"/>
-      <c r="BW5" s="2"/>
-      <c r="BX5" s="2"/>
-      <c r="BY5" s="2"/>
-      <c r="BZ5" s="2"/>
-      <c r="CA5" s="2"/>
-      <c r="CB5" s="2"/>
-      <c r="CC5" s="2"/>
-      <c r="CD5" s="2"/>
-      <c r="CE5" s="2"/>
-      <c r="CF5" s="2"/>
-      <c r="CG5" s="2"/>
-      <c r="CH5" s="2"/>
-      <c r="CI5" s="2"/>
-      <c r="CJ5" s="2"/>
-      <c r="CK5" s="2"/>
-      <c r="CL5" s="2"/>
-      <c r="CM5" s="2"/>
-      <c r="CN5" s="2"/>
-      <c r="CO5" s="2"/>
-      <c r="CP5" s="2"/>
-      <c r="CQ5" s="2"/>
-      <c r="CR5" s="2"/>
-      <c r="CS5" s="2"/>
-      <c r="CT5" s="2"/>
-      <c r="CU5" s="2"/>
-      <c r="CV5" s="2"/>
-      <c r="CW5" s="2"/>
-      <c r="CX5" s="2"/>
-      <c r="CY5" s="2"/>
-      <c r="CZ5" s="2"/>
-      <c r="DA5" s="2"/>
-      <c r="DB5" s="2"/>
-      <c r="DC5" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD5" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="DF5" s="2">
-        <v>6</v>
-      </c>
-      <c r="DG5" s="2">
-        <v>3</v>
-      </c>
-      <c r="DH5" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI5" s="2"/>
-      <c r="DJ5" s="2"/>
-      <c r="DK5" s="2"/>
-      <c r="DL5" s="2"/>
-      <c r="DM5" s="2"/>
-      <c r="DN5" s="2"/>
-      <c r="DO5" s="2"/>
-      <c r="DP5" s="2"/>
-      <c r="DQ5" s="2"/>
-      <c r="DR5" s="2"/>
-      <c r="DS5" s="2"/>
-      <c r="DT5" s="2"/>
-      <c r="DU5" s="2"/>
-      <c r="DV5" s="2"/>
-      <c r="DW5" s="2"/>
-      <c r="DX5" s="2"/>
-      <c r="DY5" s="2"/>
-      <c r="DZ5" s="2"/>
-      <c r="EA5" s="2"/>
-      <c r="EB5" s="2"/>
-      <c r="EC5" s="2"/>
-      <c r="ED5" s="2"/>
-      <c r="EE5" s="2"/>
-      <c r="EF5" s="2"/>
-      <c r="EG5" s="2"/>
-      <c r="EH5" s="2"/>
-      <c r="EI5" s="2"/>
-      <c r="EJ5" s="2"/>
-      <c r="EK5" s="2"/>
-      <c r="EL5" s="2"/>
-      <c r="EM5" s="2"/>
-      <c r="EN5" s="2"/>
-      <c r="EO5" s="2"/>
-      <c r="EP5" s="2"/>
-      <c r="EQ5" s="2"/>
-      <c r="ER5" s="2"/>
-      <c r="ES5" s="2"/>
-      <c r="ET5" s="2"/>
-      <c r="EU5" s="2"/>
-      <c r="EV5" s="2"/>
-      <c r="EW5" s="2"/>
-      <c r="EX5" s="2"/>
-      <c r="EY5" s="2"/>
-      <c r="EZ5" s="2"/>
-      <c r="FA5" s="2"/>
-      <c r="FB5" s="2"/>
-      <c r="FC5" s="2"/>
-      <c r="FD5" s="2"/>
-      <c r="FE5" s="2"/>
-      <c r="FF5" s="2"/>
-      <c r="FG5" s="2"/>
-      <c r="FH5" s="2"/>
-      <c r="FI5" s="2"/>
-      <c r="FJ5" s="2"/>
-      <c r="FK5" s="2"/>
-      <c r="FL5" s="2"/>
-      <c r="FM5" s="2"/>
-      <c r="FN5" s="2"/>
-      <c r="FO5" s="2"/>
-      <c r="FP5" s="2"/>
-      <c r="FQ5" s="2"/>
-      <c r="FR5" s="2"/>
-      <c r="FS5" s="2"/>
-      <c r="FT5" s="2"/>
-      <c r="FU5" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="FV5" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="FW5" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="FX5" s="2"/>
-      <c r="FY5" s="2"/>
-      <c r="FZ5" s="2"/>
-      <c r="GA5" s="2"/>
-      <c r="GB5" s="2"/>
-      <c r="GC5" s="2"/>
-      <c r="GD5" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE5" s="2"/>
-      <c r="GF5" s="2"/>
-      <c r="GG5" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="GH5" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R6" s="2">
-        <v>1</v>
-      </c>
-      <c r="S6" s="2">
-        <v>5</v>
-      </c>
-      <c r="T6" s="2">
-        <v>2</v>
-      </c>
-      <c r="U6" s="2">
-        <v>1</v>
-      </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X6" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD6" s="2">
-        <v>500</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>10</v>
-      </c>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>10</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="2"/>
-      <c r="AT6" s="2"/>
-      <c r="AU6" s="2"/>
-      <c r="AV6" s="2"/>
-      <c r="AW6" s="2"/>
-      <c r="AX6" s="2"/>
-      <c r="AY6" s="2"/>
-      <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
-      <c r="BB6" s="2"/>
-      <c r="BC6" s="2"/>
-      <c r="BD6" s="2"/>
-      <c r="BE6" s="2"/>
-      <c r="BF6" s="2"/>
-      <c r="BG6" s="2"/>
-      <c r="BH6" s="2"/>
-      <c r="BI6" s="2"/>
-      <c r="BJ6" s="2"/>
-      <c r="BK6" s="2"/>
-      <c r="BL6" s="2"/>
-      <c r="BM6" s="2"/>
-      <c r="BN6" s="2"/>
-      <c r="BO6" s="2"/>
-      <c r="BP6" s="2"/>
-      <c r="BQ6" s="2"/>
-      <c r="BR6" s="2"/>
-      <c r="BS6" s="2"/>
-      <c r="BT6" s="2"/>
-      <c r="BU6" s="2"/>
-      <c r="BV6" s="2"/>
-      <c r="BW6" s="2"/>
-      <c r="BX6" s="2"/>
-      <c r="BY6" s="2"/>
-      <c r="BZ6" s="2"/>
-      <c r="CA6" s="2"/>
-      <c r="CB6" s="2"/>
-      <c r="CC6" s="2"/>
-      <c r="CD6" s="2"/>
-      <c r="CE6" s="2"/>
-      <c r="CF6" s="2"/>
-      <c r="CG6" s="2"/>
-      <c r="CH6" s="2"/>
-      <c r="CI6" s="2"/>
-      <c r="CJ6" s="2"/>
-      <c r="CK6" s="2"/>
-      <c r="CL6" s="2"/>
-      <c r="CM6" s="2"/>
-      <c r="CN6" s="2"/>
-      <c r="CO6" s="2"/>
-      <c r="CP6" s="2"/>
-      <c r="CQ6" s="2"/>
-      <c r="CR6" s="2"/>
-      <c r="CS6" s="2"/>
-      <c r="CT6" s="2"/>
-      <c r="CU6" s="2"/>
-      <c r="CV6" s="2"/>
-      <c r="CW6" s="2"/>
-      <c r="CX6" s="2"/>
-      <c r="CY6" s="2"/>
-      <c r="CZ6" s="2"/>
-      <c r="DA6" s="2"/>
-      <c r="DB6" s="2"/>
-      <c r="DC6" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD6" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="DF6" s="2">
-        <v>2</v>
-      </c>
-      <c r="DG6" s="2">
-        <v>3</v>
-      </c>
-      <c r="DH6" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI6" s="2"/>
-      <c r="DJ6" s="2"/>
-      <c r="DK6" s="2"/>
-      <c r="DL6" s="2"/>
-      <c r="DM6" s="2"/>
-      <c r="DN6" s="2"/>
-      <c r="DO6" s="2"/>
-      <c r="DP6" s="2"/>
-      <c r="DQ6" s="2"/>
-      <c r="DR6" s="2"/>
-      <c r="DS6" s="2"/>
-      <c r="DT6" s="2"/>
-      <c r="DU6" s="2"/>
-      <c r="DV6" s="2"/>
-      <c r="DW6" s="2"/>
-      <c r="DX6" s="2"/>
-      <c r="DY6" s="2"/>
-      <c r="DZ6" s="2"/>
-      <c r="EA6" s="2"/>
-      <c r="EB6" s="2"/>
-      <c r="EC6" s="2"/>
-      <c r="ED6" s="2"/>
-      <c r="EE6" s="2"/>
-      <c r="EF6" s="2"/>
-      <c r="EG6" s="2"/>
-      <c r="EH6" s="2"/>
-      <c r="EI6" s="2"/>
-      <c r="EJ6" s="2"/>
-      <c r="EK6" s="2"/>
-      <c r="EL6" s="2"/>
-      <c r="EM6" s="2"/>
-      <c r="EN6" s="2"/>
-      <c r="EO6" s="2"/>
-      <c r="EP6" s="2"/>
-      <c r="EQ6" s="2"/>
-      <c r="ER6" s="2"/>
-      <c r="ES6" s="2"/>
-      <c r="ET6" s="2"/>
-      <c r="EU6" s="2"/>
-      <c r="EV6" s="2"/>
-      <c r="EW6" s="2"/>
-      <c r="EX6" s="2"/>
-      <c r="EY6" s="2"/>
-      <c r="EZ6" s="2"/>
-      <c r="FA6" s="2"/>
-      <c r="FB6" s="2"/>
-      <c r="FC6" s="2"/>
-      <c r="FD6" s="2"/>
-      <c r="FE6" s="2"/>
-      <c r="FF6" s="2"/>
-      <c r="FG6" s="2"/>
-      <c r="FH6" s="2"/>
-      <c r="FI6" s="2"/>
-      <c r="FJ6" s="2"/>
-      <c r="FK6" s="2"/>
-      <c r="FL6" s="2"/>
-      <c r="FM6" s="2"/>
-      <c r="FN6" s="2"/>
-      <c r="FO6" s="2"/>
-      <c r="FP6" s="2"/>
-      <c r="FQ6" s="2"/>
-      <c r="FR6" s="2"/>
-      <c r="FS6" s="2"/>
-      <c r="FT6" s="2"/>
-      <c r="FU6" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="FV6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="FW6" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="FX6" s="2"/>
-      <c r="FY6" s="2"/>
-      <c r="FZ6" s="2"/>
-      <c r="GA6" s="2"/>
-      <c r="GB6" s="2"/>
-      <c r="GC6" s="2"/>
-      <c r="GD6" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE6" s="2"/>
-      <c r="GF6" s="2"/>
-      <c r="GG6" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="GH6" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="T7" s="2">
-        <v>3</v>
-      </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>30</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
-      <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
-      <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
-      <c r="AV7" s="2"/>
-      <c r="AW7" s="2"/>
-      <c r="AX7" s="2"/>
-      <c r="AY7" s="2"/>
-      <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
-      <c r="BB7" s="2"/>
-      <c r="BC7" s="2"/>
-      <c r="BD7" s="2"/>
-      <c r="BE7" s="2"/>
-      <c r="BF7" s="2"/>
-      <c r="BG7" s="2"/>
-      <c r="BH7" s="2"/>
-      <c r="BI7" s="2"/>
-      <c r="BJ7" s="2"/>
-      <c r="BK7" s="2"/>
-      <c r="BL7" s="2"/>
-      <c r="BM7" s="2"/>
-      <c r="BN7" s="2"/>
-      <c r="BO7" s="2"/>
-      <c r="BP7" s="2"/>
-      <c r="BQ7" s="2"/>
-      <c r="BR7" s="2"/>
-      <c r="BS7" s="2"/>
-      <c r="BT7" s="2"/>
-      <c r="BU7" s="2"/>
-      <c r="BV7" s="2"/>
-      <c r="BW7" s="2"/>
-      <c r="BX7" s="2"/>
-      <c r="BY7" s="2"/>
-      <c r="BZ7" s="2"/>
-      <c r="CA7" s="2"/>
-      <c r="CB7" s="2"/>
-      <c r="CC7" s="2"/>
-      <c r="CD7" s="2"/>
-      <c r="CE7" s="2"/>
-      <c r="CF7" s="2"/>
-      <c r="CG7" s="2"/>
-      <c r="CH7" s="2"/>
-      <c r="CI7" s="2"/>
-      <c r="CJ7" s="2"/>
-      <c r="CK7" s="2"/>
-      <c r="CL7" s="2"/>
-      <c r="CM7" s="2"/>
-      <c r="CN7" s="2"/>
-      <c r="CO7" s="2"/>
-      <c r="CP7" s="2"/>
-      <c r="CQ7" s="2"/>
-      <c r="CR7" s="2"/>
-      <c r="CS7" s="2"/>
-      <c r="CT7" s="2"/>
-      <c r="CU7" s="2"/>
-      <c r="CV7" s="2"/>
-      <c r="CW7" s="2"/>
-      <c r="CX7" s="2"/>
-      <c r="CY7" s="2"/>
-      <c r="CZ7" s="2"/>
-      <c r="DA7" s="2"/>
-      <c r="DB7" s="2"/>
-      <c r="DC7" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD7" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="DF7" s="2">
-        <v>2</v>
-      </c>
-      <c r="DG7" s="2">
-        <v>3</v>
-      </c>
-      <c r="DH7" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI7" s="2"/>
-      <c r="DJ7" s="2"/>
-      <c r="DK7" s="2"/>
-      <c r="DL7" s="2"/>
-      <c r="DM7" s="2"/>
-      <c r="DN7" s="2"/>
-      <c r="DO7" s="2"/>
-      <c r="DP7" s="2"/>
-      <c r="DQ7" s="2"/>
-      <c r="DR7" s="2"/>
-      <c r="DS7" s="2"/>
-      <c r="DT7" s="2"/>
-      <c r="DU7" s="2"/>
-      <c r="DV7" s="2"/>
-      <c r="DW7" s="2"/>
-      <c r="DX7" s="2"/>
-      <c r="DY7" s="2"/>
-      <c r="DZ7" s="2"/>
-      <c r="EA7" s="2"/>
-      <c r="EB7" s="2"/>
-      <c r="EC7" s="2"/>
-      <c r="ED7" s="2"/>
-      <c r="EE7" s="2"/>
-      <c r="EF7" s="2"/>
-      <c r="EG7" s="2"/>
-      <c r="EH7" s="2"/>
-      <c r="EI7" s="2"/>
-      <c r="EJ7" s="2"/>
-      <c r="EK7" s="2"/>
-      <c r="EL7" s="2"/>
-      <c r="EM7" s="2"/>
-      <c r="EN7" s="2"/>
-      <c r="EO7" s="2"/>
-      <c r="EP7" s="2"/>
-      <c r="EQ7" s="2"/>
-      <c r="ER7" s="2"/>
-      <c r="ES7" s="2"/>
-      <c r="ET7" s="2"/>
-      <c r="EU7" s="2"/>
-      <c r="EV7" s="2"/>
-      <c r="EW7" s="2"/>
-      <c r="EX7" s="2"/>
-      <c r="EY7" s="2"/>
-      <c r="EZ7" s="2"/>
-      <c r="FA7" s="2"/>
-      <c r="FB7" s="2"/>
-      <c r="FC7" s="2"/>
-      <c r="FD7" s="2"/>
-      <c r="FE7" s="2"/>
-      <c r="FF7" s="2"/>
-      <c r="FG7" s="2"/>
-      <c r="FH7" s="2"/>
-      <c r="FI7" s="2"/>
-      <c r="FJ7" s="2"/>
-      <c r="FK7" s="2"/>
-      <c r="FL7" s="2"/>
-      <c r="FM7" s="2"/>
-      <c r="FN7" s="2"/>
-      <c r="FO7" s="2"/>
-      <c r="FP7" s="2"/>
-      <c r="FQ7" s="2"/>
-      <c r="FR7" s="2"/>
-      <c r="FS7" s="2"/>
-      <c r="FT7" s="2"/>
-      <c r="FU7" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="FV7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="FW7" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="FX7" s="2"/>
-      <c r="FY7" s="2"/>
-      <c r="FZ7" s="2"/>
-      <c r="GA7" s="2"/>
-      <c r="GB7" s="2"/>
-      <c r="GC7" s="2"/>
-      <c r="GD7" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE7" s="2"/>
-      <c r="GF7" s="2"/>
-      <c r="GG7" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="GH7" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R8" s="2">
-        <v>1</v>
-      </c>
-      <c r="S8" s="2">
-        <v>50</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0</v>
-      </c>
-      <c r="U8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>30</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="AE8" s="2">
-        <v>0.999</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>3</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="2"/>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
-      <c r="AV8" s="2"/>
-      <c r="AW8" s="2"/>
-      <c r="AX8" s="2"/>
-      <c r="AY8" s="2"/>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BB8" s="2"/>
-      <c r="BC8" s="2"/>
-      <c r="BD8" s="2"/>
-      <c r="BE8" s="2"/>
-      <c r="BF8" s="2"/>
-      <c r="BG8" s="2"/>
-      <c r="BH8" s="2"/>
-      <c r="BI8" s="2"/>
-      <c r="BJ8" s="2"/>
-      <c r="BK8" s="2"/>
-      <c r="BL8" s="2"/>
-      <c r="BM8" s="2"/>
-      <c r="BN8" s="2"/>
-      <c r="BO8" s="2"/>
-      <c r="BP8" s="2"/>
-      <c r="BQ8" s="2"/>
-      <c r="BR8" s="2"/>
-      <c r="BS8" s="2"/>
-      <c r="BT8" s="2"/>
-      <c r="BU8" s="2"/>
-      <c r="BV8" s="2"/>
-      <c r="BW8" s="2"/>
-      <c r="BX8" s="2"/>
-      <c r="BY8" s="2"/>
-      <c r="BZ8" s="2"/>
-      <c r="CA8" s="2"/>
-      <c r="CB8" s="2"/>
-      <c r="CC8" s="2"/>
-      <c r="CD8" s="2"/>
-      <c r="CE8" s="2"/>
-      <c r="CF8" s="2"/>
-      <c r="CG8" s="2"/>
-      <c r="CH8" s="2"/>
-      <c r="CI8" s="2"/>
-      <c r="CJ8" s="2"/>
-      <c r="CK8" s="2"/>
-      <c r="CL8" s="2"/>
-      <c r="CM8" s="2"/>
-      <c r="CN8" s="2"/>
-      <c r="CO8" s="2"/>
-      <c r="CP8" s="2"/>
-      <c r="CQ8" s="2"/>
-      <c r="CR8" s="2"/>
-      <c r="CS8" s="2"/>
-      <c r="CT8" s="2"/>
-      <c r="CU8" s="2"/>
-      <c r="CV8" s="2"/>
-      <c r="CW8" s="2"/>
-      <c r="CX8" s="2"/>
-      <c r="CY8" s="2"/>
-      <c r="CZ8" s="2"/>
-      <c r="DA8" s="2"/>
-      <c r="DB8" s="2"/>
-      <c r="DC8" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD8" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="DF8" s="2">
-        <v>2</v>
-      </c>
-      <c r="DG8" s="2">
-        <v>3</v>
-      </c>
-      <c r="DH8" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI8" s="2"/>
-      <c r="DJ8" s="2"/>
-      <c r="DK8" s="2"/>
-      <c r="DL8" s="2"/>
-      <c r="DM8" s="2"/>
-      <c r="DN8" s="2"/>
-      <c r="DO8" s="2"/>
-      <c r="DP8" s="2"/>
-      <c r="DQ8" s="2"/>
-      <c r="DR8" s="2"/>
-      <c r="DS8" s="2"/>
-      <c r="DT8" s="2"/>
-      <c r="DU8" s="2"/>
-      <c r="DV8" s="2"/>
-      <c r="DW8" s="2"/>
-      <c r="DX8" s="2"/>
-      <c r="DY8" s="2"/>
-      <c r="DZ8" s="2"/>
-      <c r="EA8" s="2"/>
-      <c r="EB8" s="2"/>
-      <c r="EC8" s="2"/>
-      <c r="ED8" s="2"/>
-      <c r="EE8" s="2"/>
-      <c r="EF8" s="2"/>
-      <c r="EG8" s="2"/>
-      <c r="EH8" s="2"/>
-      <c r="EI8" s="2"/>
-      <c r="EJ8" s="2"/>
-      <c r="EK8" s="2"/>
-      <c r="EL8" s="2"/>
-      <c r="EM8" s="2"/>
-      <c r="EN8" s="2"/>
-      <c r="EO8" s="2"/>
-      <c r="EP8" s="2"/>
-      <c r="EQ8" s="2"/>
-      <c r="ER8" s="2"/>
-      <c r="ES8" s="2"/>
-      <c r="ET8" s="2"/>
-      <c r="EU8" s="2"/>
-      <c r="EV8" s="2"/>
-      <c r="EW8" s="2"/>
-      <c r="EX8" s="2"/>
-      <c r="EY8" s="2"/>
-      <c r="EZ8" s="2"/>
-      <c r="FA8" s="2"/>
-      <c r="FB8" s="2"/>
-      <c r="FC8" s="2"/>
-      <c r="FD8" s="2"/>
-      <c r="FE8" s="2"/>
-      <c r="FF8" s="2"/>
-      <c r="FG8" s="2"/>
-      <c r="FH8" s="2"/>
-      <c r="FI8" s="2"/>
-      <c r="FJ8" s="2"/>
-      <c r="FK8" s="2"/>
-      <c r="FL8" s="2"/>
-      <c r="FM8" s="2"/>
-      <c r="FN8" s="2"/>
-      <c r="FO8" s="2"/>
-      <c r="FP8" s="2"/>
-      <c r="FQ8" s="2"/>
-      <c r="FR8" s="2"/>
-      <c r="FS8" s="2"/>
-      <c r="FT8" s="2"/>
-      <c r="FU8" s="2"/>
-      <c r="FV8" s="2"/>
-      <c r="FW8" s="2"/>
-      <c r="FX8" s="2"/>
-      <c r="FY8" s="2"/>
-      <c r="FZ8" s="2"/>
-      <c r="GA8" s="2"/>
-      <c r="GB8" s="2"/>
-      <c r="GC8" s="2"/>
-      <c r="GD8" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE8" s="2"/>
-      <c r="GF8" s="2"/>
-      <c r="GG8" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="GH8" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:190" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="R9" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="T9" s="2">
-        <v>3</v>
-      </c>
-      <c r="U9" s="2">
-        <v>1</v>
-      </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="X9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>30</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>50</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="2"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
-      <c r="AQ9" s="2"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2"/>
-      <c r="AW9" s="2"/>
-      <c r="AX9" s="2"/>
-      <c r="AY9" s="2"/>
-      <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
-      <c r="BB9" s="2"/>
-      <c r="BC9" s="2"/>
-      <c r="BD9" s="2"/>
-      <c r="BE9" s="2"/>
-      <c r="BF9" s="2"/>
-      <c r="BG9" s="2"/>
-      <c r="BH9" s="2"/>
-      <c r="BI9" s="2"/>
-      <c r="BJ9" s="2"/>
-      <c r="BK9" s="2"/>
-      <c r="BL9" s="2"/>
-      <c r="BM9" s="2"/>
-      <c r="BN9" s="2"/>
-      <c r="BO9" s="2"/>
-      <c r="BP9" s="2"/>
-      <c r="BQ9" s="2"/>
-      <c r="BR9" s="2"/>
-      <c r="BS9" s="2"/>
-      <c r="BT9" s="2"/>
-      <c r="BU9" s="2"/>
-      <c r="BV9" s="2"/>
-      <c r="BW9" s="2"/>
-      <c r="BX9" s="2"/>
-      <c r="BY9" s="2"/>
-      <c r="BZ9" s="2"/>
-      <c r="CA9" s="2"/>
-      <c r="CB9" s="2"/>
-      <c r="CC9" s="2"/>
-      <c r="CD9" s="2"/>
-      <c r="CE9" s="2"/>
-      <c r="CF9" s="2"/>
-      <c r="CG9" s="2"/>
-      <c r="CH9" s="2"/>
-      <c r="CI9" s="2"/>
-      <c r="CJ9" s="2"/>
-      <c r="CK9" s="2"/>
-      <c r="CL9" s="2"/>
-      <c r="CM9" s="2"/>
-      <c r="CN9" s="2"/>
-      <c r="CO9" s="2"/>
-      <c r="CP9" s="2"/>
-      <c r="CQ9" s="2"/>
-      <c r="CR9" s="2"/>
-      <c r="CS9" s="2"/>
-      <c r="CT9" s="2"/>
-      <c r="CU9" s="2"/>
-      <c r="CV9" s="2"/>
-      <c r="CW9" s="2"/>
-      <c r="CX9" s="2"/>
-      <c r="CY9" s="2"/>
-      <c r="CZ9" s="2"/>
-      <c r="DA9" s="2"/>
-      <c r="DB9" s="2"/>
-      <c r="DC9" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DD9" s="2">
-        <v>0</v>
-      </c>
-      <c r="DE9" s="2">
-        <v>1000</v>
-      </c>
-      <c r="DF9" s="2">
-        <v>4</v>
-      </c>
-      <c r="DG9" s="2">
-        <v>3</v>
-      </c>
-      <c r="DH9" s="2">
-        <v>1</v>
-      </c>
-      <c r="DI9" s="2"/>
-      <c r="DJ9" s="2"/>
-      <c r="DK9" s="2"/>
-      <c r="DL9" s="2"/>
-      <c r="DM9" s="2"/>
-      <c r="DN9" s="2"/>
-      <c r="DO9" s="2"/>
-      <c r="DP9" s="2"/>
-      <c r="DQ9" s="2"/>
-      <c r="DR9" s="2"/>
-      <c r="DS9" s="2"/>
-      <c r="DT9" s="2"/>
-      <c r="DU9" s="2"/>
-      <c r="DV9" s="2"/>
-      <c r="DW9" s="2"/>
-      <c r="DX9" s="2"/>
-      <c r="DY9" s="2"/>
-      <c r="DZ9" s="2"/>
-      <c r="EA9" s="2"/>
-      <c r="EB9" s="2"/>
-      <c r="EC9" s="2"/>
-      <c r="ED9" s="2"/>
-      <c r="EE9" s="2"/>
-      <c r="EF9" s="2"/>
-      <c r="EG9" s="2"/>
-      <c r="EH9" s="2"/>
-      <c r="EI9" s="2"/>
-      <c r="EJ9" s="2"/>
-      <c r="EK9" s="2"/>
-      <c r="EL9" s="2"/>
-      <c r="EM9" s="2"/>
-      <c r="EN9" s="2"/>
-      <c r="EO9" s="2"/>
-      <c r="EP9" s="2"/>
-      <c r="EQ9" s="2"/>
-      <c r="ER9" s="2"/>
-      <c r="ES9" s="2"/>
-      <c r="ET9" s="2"/>
-      <c r="EU9" s="2"/>
-      <c r="EV9" s="2"/>
-      <c r="EW9" s="2"/>
-      <c r="EX9" s="2"/>
-      <c r="EY9" s="2"/>
-      <c r="EZ9" s="2"/>
-      <c r="FA9" s="2"/>
-      <c r="FB9" s="2"/>
-      <c r="FC9" s="2"/>
-      <c r="FD9" s="2"/>
-      <c r="FE9" s="2"/>
-      <c r="FF9" s="2"/>
-      <c r="FG9" s="2"/>
-      <c r="FH9" s="2"/>
-      <c r="FI9" s="2"/>
-      <c r="FJ9" s="2"/>
-      <c r="FK9" s="2"/>
-      <c r="FL9" s="2"/>
-      <c r="FM9" s="2"/>
-      <c r="FN9" s="2"/>
-      <c r="FO9" s="2"/>
-      <c r="FP9" s="2"/>
-      <c r="FQ9" s="2"/>
-      <c r="FR9" s="2"/>
-      <c r="FS9" s="2"/>
-      <c r="FT9" s="2"/>
-      <c r="FU9" s="2"/>
-      <c r="FV9" s="2"/>
-      <c r="FW9" s="2"/>
-      <c r="FX9" s="2"/>
-      <c r="FY9" s="2"/>
-      <c r="FZ9" s="2"/>
-      <c r="GA9" s="2"/>
-      <c r="GB9" s="2"/>
-      <c r="GC9" s="2"/>
-      <c r="GD9" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="GE9" s="2"/>
-      <c r="GF9" s="2"/>
-      <c r="GG9" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="GH9" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>